<commit_message>
Changing my concept again
</commit_message>
<xml_diff>
--- a/Pin Brainstorming deej.xlsx
+++ b/Pin Brainstorming deej.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikla\Documents\GitHub\deejWithButtons\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikla\Documents\GitHub\deej\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD9C8FB-45C1-4649-9D18-DA3F8FB725D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B498361B-5BC5-40FA-9DCA-6773CC5AA708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{320EC7C1-8A55-4CF7-B81F-562E306DE035}"/>
   </bookViews>
@@ -652,7 +652,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -810,14 +810,14 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="2">
@@ -853,14 +853,14 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>7</v>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="2">

</xml_diff>

<commit_message>
Doing some weird stuff
</commit_message>
<xml_diff>
--- a/Pin Brainstorming deej.xlsx
+++ b/Pin Brainstorming deej.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikla\Documents\GitHub\deej\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B498361B-5BC5-40FA-9DCA-6773CC5AA708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C0B6E6-7BD0-4BF6-A706-0545892A7127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{320EC7C1-8A55-4CF7-B81F-562E306DE035}"/>
   </bookViews>
@@ -294,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -333,6 +333,12 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -652,7 +658,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -756,11 +762,11 @@
         <v>1</v>
       </c>
       <c r="N2" s="8">
-        <v>11.9</v>
+        <v>10</v>
       </c>
       <c r="O2" s="8">
         <f>PRODUCT(M2, N2)</f>
-        <v>11.9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -792,18 +798,18 @@
       <c r="J3" s="2">
         <v>4220</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="L3" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="M3" s="13">
+      <c r="M3" s="15">
         <v>1</v>
       </c>
-      <c r="N3" s="8">
-        <v>8</v>
-      </c>
-      <c r="O3" s="8">
+      <c r="N3" s="14">
+        <v>0</v>
+      </c>
+      <c r="O3" s="14">
         <f>PRODUCT(M3, N3)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -842,11 +848,11 @@
         <v>6</v>
       </c>
       <c r="N4" s="8">
-        <v>6.99</v>
+        <v>5.87</v>
       </c>
       <c r="O4" s="8">
         <f t="shared" ref="O4:O9" si="0">PRODUCT(M4, N4)</f>
-        <v>41.94</v>
+        <v>35.22</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -891,6 +897,9 @@
         <f t="shared" si="0"/>
         <v>8.94</v>
       </c>
+      <c r="P5" s="8" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -928,14 +937,11 @@
         <v>6</v>
       </c>
       <c r="N6" s="8">
-        <v>2.29</v>
+        <v>1.92</v>
       </c>
       <c r="O6" s="8">
         <f t="shared" si="0"/>
-        <v>13.74</v>
-      </c>
-      <c r="P6" s="8" t="s">
-        <v>43</v>
+        <v>11.52</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
@@ -1026,7 +1032,7 @@
       </c>
       <c r="O11" s="8">
         <f>SUM(O2:O9)</f>
-        <v>101.30999999999999</v>
+        <v>82.469999999999985</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Overengineering the arduino stuff
</commit_message>
<xml_diff>
--- a/Pin Brainstorming deej.xlsx
+++ b/Pin Brainstorming deej.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikla\Documents\GitHub\deej\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C0B6E6-7BD0-4BF6-A706-0545892A7127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B49145-3B0B-4CF0-B67F-6A457FFE417E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{320EC7C1-8A55-4CF7-B81F-562E306DE035}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
   <si>
     <t>Slider</t>
   </si>
@@ -167,12 +167,6 @@
     <t>Color</t>
   </si>
   <si>
-    <t>4 Schwarz; 1 Grau, 1 Rot</t>
-  </si>
-  <si>
-    <t>Stück</t>
-  </si>
-  <si>
     <t>Anzahl</t>
   </si>
   <si>
@@ -185,20 +179,50 @@
     <t xml:space="preserve">Knopf </t>
   </si>
   <si>
-    <t xml:space="preserve">Wiederstand </t>
-  </si>
-  <si>
     <t>Display</t>
   </si>
   <si>
-    <t>7-Segment</t>
+    <t xml:space="preserve">Widerstand </t>
+  </si>
+  <si>
+    <t>EAN</t>
+  </si>
+  <si>
+    <t>C-4250236822907</t>
+  </si>
+  <si>
+    <t>C-2050000114397</t>
+  </si>
+  <si>
+    <t>C-2050000113758</t>
+  </si>
+  <si>
+    <t>C-2050004878899</t>
+  </si>
+  <si>
+    <t>C-2050000096181</t>
+  </si>
+  <si>
+    <t>Stück (€)</t>
+  </si>
+  <si>
+    <t>Schwarz</t>
+  </si>
+  <si>
+    <t>Rot</t>
+  </si>
+  <si>
+    <t>C-2050000113789</t>
+  </si>
+  <si>
+    <t>Lever 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,6 +245,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -277,7 +308,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.499984740745262"/>
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -294,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -329,9 +360,6 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -339,6 +367,12 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -655,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4227582-90D1-41E2-AB66-426EF4C42A3D}">
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -678,11 +712,12 @@
     <col min="13" max="13" width="8.88671875" customWidth="1"/>
     <col min="14" max="14" width="11.5546875" style="8"/>
     <col min="15" max="15" width="7.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.77734375" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="11.5546875" style="8"/>
+    <col min="16" max="16" width="7.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.5546875" style="8" customWidth="1"/>
+    <col min="18" max="16384" width="11.5546875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -717,16 +752,19 @@
         <v>37</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="O1" s="7" t="s">
         <v>38</v>
       </c>
+      <c r="Q1" s="7" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -739,7 +777,7 @@
       <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="12"/>
+      <c r="E2" s="15"/>
       <c r="F2" s="2">
         <v>1</v>
       </c>
@@ -758,18 +796,21 @@
       <c r="L2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="M2" s="13">
+      <c r="M2" s="12">
         <v>1</v>
       </c>
       <c r="N2" s="8">
-        <v>10</v>
+        <v>11.9</v>
       </c>
       <c r="O2" s="8">
         <f>PRODUCT(M2, N2)</f>
-        <v>10</v>
+        <v>11.9</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -798,21 +839,21 @@
       <c r="J3" s="2">
         <v>4220</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="L3" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="M3" s="15">
+      <c r="M3" s="14">
         <v>1</v>
       </c>
-      <c r="N3" s="14">
+      <c r="N3" s="13">
         <v>0</v>
       </c>
-      <c r="O3" s="14">
+      <c r="O3" s="13">
         <f>PRODUCT(M3, N3)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -842,20 +883,26 @@
         <v>4221</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="M4" s="13">
+        <v>44</v>
+      </c>
+      <c r="M4" s="12">
         <v>6</v>
       </c>
       <c r="N4" s="8">
-        <v>5.87</v>
+        <v>6.99</v>
       </c>
       <c r="O4" s="8">
-        <f t="shared" ref="O4:O9" si="0">PRODUCT(M4, N4)</f>
-        <v>35.22</v>
+        <f t="shared" ref="O4:O8" si="0">PRODUCT(M4, N4)</f>
+        <v>41.94</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -885,23 +932,26 @@
         <v>4222</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="M5" s="13">
-        <v>6</v>
+        <v>45</v>
+      </c>
+      <c r="M5" s="12">
+        <v>4</v>
       </c>
       <c r="N5" s="8">
         <v>1.49</v>
       </c>
       <c r="O5" s="8">
-        <f t="shared" si="0"/>
-        <v>8.94</v>
+        <f>PRODUCT(M5, N5)</f>
+        <v>5.96</v>
       </c>
       <c r="P5" s="8" t="s">
-        <v>43</v>
+        <v>56</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -931,20 +981,26 @@
         <v>4223</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M6" s="13">
-        <v>6</v>
+        <v>45</v>
+      </c>
+      <c r="M6" s="12">
+        <v>2</v>
       </c>
       <c r="N6" s="8">
-        <v>1.92</v>
+        <v>1.49</v>
       </c>
       <c r="O6" s="8">
-        <f t="shared" si="0"/>
-        <v>11.52</v>
+        <f>PRODUCT(M6, N6)</f>
+        <v>2.98</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -974,65 +1030,74 @@
         <v>4224</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="M7" s="13">
+        <v>46</v>
+      </c>
+      <c r="M7" s="12">
         <v>6</v>
       </c>
       <c r="N7" s="8">
-        <v>0.05</v>
+        <v>2.29</v>
       </c>
       <c r="O7" s="8">
-        <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
+        <f>PRODUCT(M7, N7)</f>
+        <v>13.74</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="L8" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="M8" s="13">
-        <v>1</v>
+        <v>48</v>
+      </c>
+      <c r="M8" s="12">
+        <v>6</v>
       </c>
       <c r="N8" s="8">
-        <v>9</v>
+        <v>0.05</v>
       </c>
       <c r="O8" s="8">
-        <f t="shared" si="0"/>
-        <v>9</v>
+        <f>PRODUCT(M8, N8)</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="Q8" s="8" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
-      <c r="L9" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="M9" s="13">
+      <c r="L9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="M9" s="16">
         <v>1</v>
       </c>
-      <c r="N9" s="8">
-        <v>7.49</v>
-      </c>
-      <c r="O9" s="8">
-        <f t="shared" si="0"/>
-        <v>7.49</v>
+      <c r="N9" s="6">
+        <v>0</v>
+      </c>
+      <c r="O9" s="6">
+        <f>PRODUCT(M9, N9)</f>
+        <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="M10" s="12"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="L11" s="8" t="s">
         <v>41</v>
       </c>
       <c r="O11" s="8">
         <f>SUM(O2:O9)</f>
-        <v>82.469999999999985</v>
+        <v>76.819999999999993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Pin Brainstorming deej.xlsx
</commit_message>
<xml_diff>
--- a/Pin Brainstorming deej.xlsx
+++ b/Pin Brainstorming deej.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikla\Documents\GitHub\deej\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B49145-3B0B-4CF0-B67F-6A457FFE417E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8A70F8-DBEF-4C3B-A3F2-00D94235CAEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{320EC7C1-8A55-4CF7-B81F-562E306DE035}"/>
   </bookViews>
@@ -692,7 +692,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -892,7 +892,7 @@
         <v>6.99</v>
       </c>
       <c r="O4" s="8">
-        <f t="shared" ref="O4:O8" si="0">PRODUCT(M4, N4)</f>
+        <f t="shared" ref="O4" si="0">PRODUCT(M4, N4)</f>
         <v>41.94</v>
       </c>
       <c r="P4" s="8" t="s">

</xml_diff>

<commit_message>
Adding a display concept
</commit_message>
<xml_diff>
--- a/Pin Brainstorming deej.xlsx
+++ b/Pin Brainstorming deej.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikla\Documents\GitHub\deej\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8A70F8-DBEF-4C3B-A3F2-00D94235CAEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEAD508D-009E-4259-A7F8-F1CAC78A0D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{320EC7C1-8A55-4CF7-B81F-562E306DE035}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
   <si>
     <t>Slider</t>
   </si>
@@ -216,6 +216,9 @@
   </si>
   <si>
     <t>Lever 1</t>
+  </si>
+  <si>
+    <t>C-4250236809434</t>
   </si>
 </sst>
 </file>
@@ -325,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -372,7 +375,10 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -692,7 +698,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1074,18 +1080,21 @@
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
-      <c r="L9" s="6" t="s">
+      <c r="L9" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="M9" s="16">
+      <c r="M9" s="17">
         <v>1</v>
       </c>
-      <c r="N9" s="6">
-        <v>0</v>
-      </c>
-      <c r="O9" s="6">
+      <c r="N9" s="16">
+        <v>9.99</v>
+      </c>
+      <c r="O9" s="16">
         <f>PRODUCT(M9, N9)</f>
-        <v>0</v>
+        <v>9.99</v>
+      </c>
+      <c r="Q9" s="8" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
@@ -1097,7 +1106,7 @@
       </c>
       <c r="O11" s="8">
         <f>SUM(O2:O9)</f>
-        <v>76.819999999999993</v>
+        <v>86.809999999999988</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed some thing in preparation to ordering an arduino micro
</commit_message>
<xml_diff>
--- a/Pin Brainstorming deej.xlsx
+++ b/Pin Brainstorming deej.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikla\Documents\GitHub\deej\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B0B95E-27C6-40B2-BC47-0BE5FA985331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63134A98-D866-4EF3-B6A1-C700AF6E3E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{320EC7C1-8A55-4CF7-B81F-562E306DE035}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
   <si>
     <t>Slider</t>
   </si>
@@ -98,12 +98,6 @@
     <t>A3</t>
   </si>
   <si>
-    <t>A6</t>
-  </si>
-  <si>
-    <t>A7</t>
-  </si>
-  <si>
     <t>Button</t>
   </si>
   <si>
@@ -155,9 +149,6 @@
     <t>Preis (€)</t>
   </si>
   <si>
-    <t>Arduino Pro Micro</t>
-  </si>
-  <si>
     <t>Kabel</t>
   </si>
   <si>
@@ -222,6 +213,21 @@
   </si>
   <si>
     <t>C-2050000113840</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>Input Pin</t>
+  </si>
+  <si>
+    <t>Output Pin</t>
+  </si>
+  <si>
+    <t>Arduino Micro</t>
   </si>
 </sst>
 </file>
@@ -263,7 +269,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -324,6 +330,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -337,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -382,6 +394,12 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -698,35 +716,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4227582-90D1-41E2-AB66-426EF4C42A3D}">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.5546875" style="8"/>
     <col min="2" max="2" width="16" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="8"/>
-    <col min="4" max="4" width="14.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" style="8"/>
-    <col min="6" max="6" width="10.88671875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="20.21875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" style="8" customWidth="1"/>
-    <col min="9" max="9" width="9.77734375" style="8" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" style="8" customWidth="1"/>
-    <col min="11" max="11" width="11" style="8" customWidth="1"/>
-    <col min="12" max="12" width="16.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.88671875" customWidth="1"/>
-    <col min="14" max="14" width="10" style="8" customWidth="1"/>
-    <col min="15" max="15" width="7.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.5546875" style="8" customWidth="1"/>
-    <col min="18" max="16384" width="11.5546875" style="8"/>
+    <col min="3" max="4" width="11.5546875" style="8"/>
+    <col min="5" max="5" width="14.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" style="8"/>
+    <col min="7" max="7" width="10.88671875" style="8" customWidth="1"/>
+    <col min="8" max="8" width="20.21875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="9.77734375" style="8" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" style="8" customWidth="1"/>
+    <col min="12" max="12" width="11" style="8" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" customWidth="1"/>
+    <col min="15" max="15" width="10" style="8" customWidth="1"/>
+    <col min="16" max="16" width="7.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.5546875" style="8" customWidth="1"/>
+    <col min="19" max="16384" width="11.5546875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -734,46 +750,49 @@
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>27</v>
-      </c>
       <c r="J1" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>37</v>
+        <v>25</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>49</v>
+        <v>52</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -783,43 +802,46 @@
       <c r="C2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="1">
         <v>9</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="2">
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="14"/>
+      <c r="G2" s="2">
         <v>1</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="2">
+      <c r="H2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="2">
+        <v>13</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="2">
         <v>4219</v>
       </c>
-      <c r="L2" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="M2" s="11">
+      <c r="M2" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="N2" s="11">
         <v>1</v>
       </c>
-      <c r="N2" s="8">
+      <c r="O2" s="8">
         <v>11.9</v>
       </c>
-      <c r="O2" s="8">
-        <f>PRODUCT(M2, N2)</f>
+      <c r="P2" s="8">
+        <f>PRODUCT(N2, O2)</f>
         <v>11.9</v>
       </c>
-      <c r="Q2" s="8" t="s">
-        <v>50</v>
+      <c r="R2" s="8" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -829,43 +851,46 @@
       <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="1">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="2">
+      <c r="F3" s="10"/>
+      <c r="G3" s="2">
         <v>2</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="2">
+      <c r="H3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="2">
+        <v>12</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="2">
+        <v>4220</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" s="13">
         <v>1</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="2">
-        <v>4220</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="M3" s="13">
-        <v>1</v>
-      </c>
-      <c r="N3" s="12">
-        <v>0</v>
-      </c>
       <c r="O3" s="12">
-        <f>PRODUCT(M3, N3)</f>
-        <v>0</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>59</v>
+        <v>0</v>
+      </c>
+      <c r="P3" s="12">
+        <f>PRODUCT(N3, O3)</f>
+        <v>0</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -875,46 +900,49 @@
       <c r="C4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="1">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="2">
+      <c r="F4" s="10"/>
+      <c r="G4" s="2">
         <v>3</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" s="2">
-        <v>2</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="2">
+      <c r="H4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="2">
+        <v>11</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="2">
         <v>4221</v>
       </c>
-      <c r="L4" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="M4" s="11">
-        <v>6</v>
-      </c>
-      <c r="N4" s="8">
+      <c r="M4" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="N4" s="11">
+        <v>5</v>
+      </c>
+      <c r="O4" s="8">
         <v>7.49</v>
       </c>
-      <c r="O4" s="8">
-        <f t="shared" ref="O4" si="0">PRODUCT(M4, N4)</f>
-        <v>44.94</v>
-      </c>
-      <c r="P4" s="8" t="s">
-        <v>57</v>
+      <c r="P4" s="8">
+        <f t="shared" ref="P4" si="0">PRODUCT(N4, O4)</f>
+        <v>37.450000000000003</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>51</v>
+        <v>54</v>
+      </c>
+      <c r="R4" s="8" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -924,46 +952,49 @@
       <c r="C5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="1">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="2">
+      <c r="F5" s="10"/>
+      <c r="G5" s="2">
         <v>4</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="2">
-        <v>3</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J5" s="2">
+      <c r="H5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="2">
+        <v>10</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" s="2">
         <v>4222</v>
       </c>
-      <c r="L5" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="M5" s="11">
-        <v>4</v>
-      </c>
-      <c r="N5" s="8">
+      <c r="M5" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="N5" s="11">
+        <v>0</v>
+      </c>
+      <c r="O5" s="8">
         <v>1.49</v>
       </c>
-      <c r="O5" s="8">
-        <f>PRODUCT(M5, N5)</f>
-        <v>5.96</v>
-      </c>
-      <c r="P5" s="8" t="s">
-        <v>56</v>
+      <c r="P5" s="8">
+        <f>PRODUCT(N5, O5)</f>
+        <v>0</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="R5" s="8" t="s">
+        <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -971,48 +1002,51 @@
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="1">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="2">
+      <c r="F6" s="10"/>
+      <c r="G6" s="2">
         <v>5</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" s="2">
-        <v>5</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" s="2">
+      <c r="H6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="2">
+        <v>3</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="2">
         <v>4223</v>
       </c>
-      <c r="L6" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="M6" s="11">
-        <v>2</v>
-      </c>
-      <c r="N6" s="8">
+      <c r="M6" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="N6" s="11">
+        <v>0</v>
+      </c>
+      <c r="O6" s="8">
         <v>1.49</v>
       </c>
-      <c r="O6" s="8">
-        <f>PRODUCT(M6, N6)</f>
-        <v>2.98</v>
-      </c>
-      <c r="P6" s="8" t="s">
-        <v>60</v>
+      <c r="P6" s="8">
+        <f>PRODUCT(N6, O6)</f>
+        <v>0</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
+      </c>
+      <c r="R6" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1020,99 +1054,102 @@
         <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="1">
+        <v>4</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="2">
+      <c r="F7" s="15"/>
+      <c r="G7" s="2">
         <v>6</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" s="2">
-        <v>7</v>
-      </c>
-      <c r="I7" s="2" t="s">
+      <c r="H7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J7" s="2">
+      <c r="I7" s="2">
+        <v>2</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="2">
         <v>4224</v>
       </c>
-      <c r="L7" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="M7" s="11">
-        <v>6</v>
-      </c>
-      <c r="N7" s="8">
+      <c r="M7" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="N7" s="11">
+        <v>0</v>
+      </c>
+      <c r="O7" s="8">
         <v>2.29</v>
       </c>
-      <c r="O7" s="8">
-        <f>PRODUCT(M7, N7)</f>
-        <v>13.74</v>
-      </c>
-      <c r="Q7" s="8" t="s">
-        <v>53</v>
+      <c r="P7" s="8">
+        <f>PRODUCT(N7, O7)</f>
+        <v>0</v>
+      </c>
+      <c r="R7" s="8" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="F8" s="9"/>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
-      <c r="L8" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M8" s="11">
-        <v>6</v>
-      </c>
-      <c r="N8" s="8">
+      <c r="J8" s="9"/>
+      <c r="M8" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="N8" s="11">
+        <v>0</v>
+      </c>
+      <c r="O8" s="8">
         <v>0.05</v>
       </c>
-      <c r="O8" s="8">
-        <f>PRODUCT(M8, N8)</f>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="Q8" s="8" t="s">
-        <v>54</v>
+      <c r="P8" s="8">
+        <f>PRODUCT(N8, O8)</f>
+        <v>0</v>
+      </c>
+      <c r="R8" s="8" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="E9" s="9"/>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
-      <c r="L9" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="M9" s="11">
-        <v>1</v>
-      </c>
-      <c r="N9" s="8">
+      <c r="J9" s="9"/>
+      <c r="M9" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="N9" s="11">
+        <v>0</v>
+      </c>
+      <c r="O9" s="8">
         <v>9.99</v>
       </c>
-      <c r="O9" s="8">
-        <f>PRODUCT(M9, N9)</f>
-        <v>9.99</v>
-      </c>
-      <c r="Q9" s="8" t="s">
-        <v>58</v>
+      <c r="P9" s="8">
+        <f>PRODUCT(N9, O9)</f>
+        <v>0</v>
+      </c>
+      <c r="R9" s="8" t="s">
+        <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="M10" s="11"/>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="N10" s="11"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="L11" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="O11" s="8">
-        <f>SUM(O2:O9)</f>
-        <v>89.809999999999988</v>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="M11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="P11" s="8">
+        <f>SUM(P2:P9)</f>
+        <v>49.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testing the arduino and display and write programs for it
</commit_message>
<xml_diff>
--- a/Pin Brainstorming deej.xlsx
+++ b/Pin Brainstorming deej.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikla\Documents\GitHub\deej\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA98D88-26D0-4EB1-BED4-BDF15D8CF5A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E058B953-D3E0-4B4B-8AEA-A4C1AB130D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{320EC7C1-8A55-4CF7-B81F-562E306DE035}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{320EC7C1-8A55-4CF7-B81F-562E306DE035}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="78">
   <si>
     <t>Slider</t>
   </si>
@@ -228,6 +228,48 @@
   </si>
   <si>
     <t>MEDIA_PREVIOUS_TRACK</t>
+  </si>
+  <si>
+    <t>C-2050000114243</t>
+  </si>
+  <si>
+    <t>Lever-T</t>
+  </si>
+  <si>
+    <t>Display Pins</t>
+  </si>
+  <si>
+    <t>VCC</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t>SCL</t>
+  </si>
+  <si>
+    <t>SDA</t>
+  </si>
+  <si>
+    <t>RS/DC</t>
+  </si>
+  <si>
+    <t>RES</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>ICSP SCK</t>
+  </si>
+  <si>
+    <t>ICSP COPI</t>
+  </si>
+  <si>
+    <t>ICSP 5V</t>
+  </si>
+  <si>
+    <t>ICSP GND</t>
   </si>
 </sst>
 </file>
@@ -349,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -398,6 +440,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -713,7 +764,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4227582-90D1-41E2-AB66-426EF4C42A3D}">
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:U12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -728,18 +779,20 @@
     <col min="8" max="8" width="20.21875" style="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.33203125" style="8" customWidth="1"/>
     <col min="10" max="10" width="22.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" style="8" customWidth="1"/>
-    <col min="12" max="12" width="11" style="8" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" customWidth="1"/>
-    <col min="15" max="15" width="10" style="8" customWidth="1"/>
-    <col min="16" max="16" width="7.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.5546875" style="8" customWidth="1"/>
-    <col min="19" max="16384" width="11.5546875" style="8"/>
+    <col min="11" max="12" width="10.33203125" style="8" customWidth="1"/>
+    <col min="13" max="13" width="11.21875" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.21875" style="8" customWidth="1"/>
+    <col min="15" max="15" width="11" style="8" customWidth="1"/>
+    <col min="16" max="16" width="16.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.88671875" customWidth="1"/>
+    <col min="18" max="18" width="10" style="8" customWidth="1"/>
+    <col min="19" max="19" width="7.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.5546875" style="8" customWidth="1"/>
+    <col min="22" max="16384" width="11.5546875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -774,22 +827,25 @@
         <v>28</v>
       </c>
       <c r="M1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="P1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -800,7 +856,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>9</v>
@@ -821,24 +877,30 @@
       <c r="K2" s="2">
         <v>4268</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="P2" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="N2" s="11">
-        <v>1</v>
-      </c>
-      <c r="O2" s="8">
+      <c r="Q2" s="11">
+        <v>0</v>
+      </c>
+      <c r="R2" s="8">
         <v>11.9</v>
       </c>
-      <c r="P2" s="8">
-        <f>PRODUCT(N2, O2)</f>
-        <v>11.9</v>
-      </c>
-      <c r="R2" s="8" t="s">
+      <c r="S2" s="8">
+        <f>PRODUCT(Q2, R2)</f>
+        <v>0</v>
+      </c>
+      <c r="U2" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -849,7 +911,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>11</v>
@@ -870,24 +932,30 @@
       <c r="K3" s="2">
         <v>4219</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="M3" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="N3" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="P3" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="N3" s="13">
+      <c r="Q3" s="13">
         <v>1</v>
       </c>
-      <c r="O3" s="12">
-        <v>0</v>
-      </c>
-      <c r="P3" s="12">
-        <f>PRODUCT(N3, O3)</f>
-        <v>0</v>
-      </c>
-      <c r="R3" s="8" t="s">
+      <c r="R3" s="12">
+        <v>0</v>
+      </c>
+      <c r="S3" s="12">
+        <f>PRODUCT(Q3, R3)</f>
+        <v>0</v>
+      </c>
+      <c r="U3" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -898,7 +966,7 @@
         <v>18</v>
       </c>
       <c r="D4" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>13</v>
@@ -919,27 +987,33 @@
       <c r="K4" s="2">
         <v>4271</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="M4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="N4" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="P4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="N4" s="11">
-        <v>5</v>
-      </c>
-      <c r="O4" s="8">
+      <c r="Q4" s="11">
+        <v>0</v>
+      </c>
+      <c r="R4" s="8">
         <v>7.49</v>
       </c>
-      <c r="P4" s="8">
-        <f t="shared" ref="P4" si="0">PRODUCT(N4, O4)</f>
-        <v>37.450000000000003</v>
-      </c>
-      <c r="Q4" s="8" t="s">
+      <c r="S4" s="8">
+        <f t="shared" ref="S4" si="0">PRODUCT(Q4, R4)</f>
+        <v>0</v>
+      </c>
+      <c r="T4" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="R4" s="8" t="s">
+      <c r="U4" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -950,7 +1024,7 @@
         <v>19</v>
       </c>
       <c r="D5" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>12</v>
@@ -963,7 +1037,7 @@
         <v>21</v>
       </c>
       <c r="I5" s="2">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>62</v>
@@ -971,27 +1045,33 @@
       <c r="K5" s="2">
         <v>4274</v>
       </c>
-      <c r="M5" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="N5" s="11">
-        <v>0</v>
-      </c>
-      <c r="O5" s="8">
-        <v>1.49</v>
-      </c>
-      <c r="P5" s="8">
-        <f>PRODUCT(N5, O5)</f>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="R5" s="8" t="s">
-        <v>45</v>
+      <c r="M5" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="N5" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q5" s="11">
+        <v>5</v>
+      </c>
+      <c r="R5" s="8">
+        <v>21.39</v>
+      </c>
+      <c r="S5" s="8">
+        <f t="shared" ref="S5:S10" si="1">PRODUCT(Q5, R5)</f>
+        <v>106.95</v>
+      </c>
+      <c r="T5" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="U5" s="8" t="s">
+        <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1002,7 +1082,7 @@
         <v>55</v>
       </c>
       <c r="D6" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>14</v>
@@ -1015,7 +1095,7 @@
         <v>22</v>
       </c>
       <c r="I6" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>63</v>
@@ -1023,27 +1103,33 @@
       <c r="K6" s="2">
         <v>4272</v>
       </c>
-      <c r="M6" s="16" t="s">
+      <c r="M6" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="N6" s="4">
+        <v>2</v>
+      </c>
+      <c r="P6" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="N6" s="11">
-        <v>0</v>
-      </c>
-      <c r="O6" s="8">
+      <c r="Q6" s="11">
+        <v>0</v>
+      </c>
+      <c r="R6" s="8">
         <v>1.49</v>
       </c>
-      <c r="P6" s="8">
-        <f>PRODUCT(N6, O6)</f>
-        <v>0</v>
-      </c>
-      <c r="Q6" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="R6" s="8" t="s">
-        <v>54</v>
+      <c r="S6" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="U6" s="8" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1054,7 +1140,7 @@
         <v>56</v>
       </c>
       <c r="D7" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>10</v>
@@ -1067,7 +1153,7 @@
         <v>29</v>
       </c>
       <c r="I7" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>27</v>
@@ -1075,82 +1161,116 @@
       <c r="K7" s="2">
         <v>4220</v>
       </c>
-      <c r="M7" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="N7" s="11">
-        <v>0</v>
-      </c>
-      <c r="O7" s="8">
-        <v>2.29</v>
-      </c>
-      <c r="P7" s="8">
-        <f>PRODUCT(N7, O7)</f>
-        <v>0</v>
-      </c>
-      <c r="R7" s="8" t="s">
-        <v>46</v>
+      <c r="M7" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="N7" s="4">
+        <v>3</v>
+      </c>
+      <c r="P7" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q7" s="11">
+        <v>0</v>
+      </c>
+      <c r="R7" s="8">
+        <v>1.49</v>
+      </c>
+      <c r="S7" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T7" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="U7" s="8" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
-      <c r="M8" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="N8" s="11">
-        <v>0</v>
-      </c>
-      <c r="O8" s="8">
-        <v>0.05</v>
-      </c>
-      <c r="P8" s="8">
-        <f>PRODUCT(N8, O8)</f>
-        <v>0</v>
-      </c>
-      <c r="R8" s="8" t="s">
-        <v>47</v>
+      <c r="M8" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="N8" s="4">
+        <v>4</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q8" s="11">
+        <v>0</v>
+      </c>
+      <c r="R8" s="8">
+        <v>2.29</v>
+      </c>
+      <c r="S8" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U8" s="8" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
-      <c r="M9" s="16" t="s">
+      <c r="P9" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q9" s="11">
+        <v>0</v>
+      </c>
+      <c r="R9" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="S9" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U9" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="P10" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="N9" s="11">
-        <v>0</v>
-      </c>
-      <c r="O9" s="8">
+      <c r="Q10" s="11">
+        <v>0</v>
+      </c>
+      <c r="R10" s="8">
         <v>9.99</v>
       </c>
-      <c r="P9" s="8">
-        <f>PRODUCT(N9, O9)</f>
-        <v>0</v>
-      </c>
-      <c r="R9" s="8" t="s">
+      <c r="S10" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U10" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="N10" s="11"/>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="Q11" s="11"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="M11" s="8" t="s">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="P12" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="P11" s="8">
-        <f>SUM(P2:P9)</f>
-        <v>49.35</v>
+      <c r="S12" s="8">
+        <f>SUM(S2:S10)</f>
+        <v>106.95</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Deej script now compiles, Buttons and screen work
</commit_message>
<xml_diff>
--- a/Pin Brainstorming deej.xlsx
+++ b/Pin Brainstorming deej.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikla\Documents\GitHub\deej\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E058B953-D3E0-4B4B-8AEA-A4C1AB130D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DD4942-CBE8-441C-A373-D8849D2C2FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{320EC7C1-8A55-4CF7-B81F-562E306DE035}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{320EC7C1-8A55-4CF7-B81F-562E306DE035}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -766,7 +766,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4227582-90D1-41E2-AB66-426EF4C42A3D}">
   <dimension ref="A1:U12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -856,7 +858,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>9</v>
@@ -911,7 +913,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>11</v>
@@ -966,7 +968,7 @@
         <v>18</v>
       </c>
       <c r="D4" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>13</v>
@@ -1024,7 +1026,7 @@
         <v>19</v>
       </c>
       <c r="D5" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>12</v>
@@ -1037,7 +1039,7 @@
         <v>21</v>
       </c>
       <c r="I5" s="2">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>62</v>
@@ -1082,7 +1084,7 @@
         <v>55</v>
       </c>
       <c r="D6" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>14</v>
@@ -1140,7 +1142,7 @@
         <v>56</v>
       </c>
       <c r="D7" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>10</v>
@@ -1196,7 +1198,7 @@
         <v>73</v>
       </c>
       <c r="N8" s="4">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="P8" s="16" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Changing the current apps works now
</commit_message>
<xml_diff>
--- a/Pin Brainstorming deej.xlsx
+++ b/Pin Brainstorming deej.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikla\Documents\GitHub\deej\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D947E22D-6C88-46E4-AA2A-0630DBD08E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938FD238-5B77-4D3D-A40D-F04084A9ADB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{320EC7C1-8A55-4CF7-B81F-562E306DE035}"/>
   </bookViews>
@@ -766,9 +766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4227582-90D1-41E2-AB66-426EF4C42A3D}">
   <dimension ref="A1:U12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>